<commit_message>
Some validations are added...
</commit_message>
<xml_diff>
--- a/TestData/secondFlow/addVcenter.xlsx
+++ b/TestData/secondFlow/addVcenter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\secondFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A828FF6-7E3A-47C7-9233-8FF6B7F17B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E91C3E5-3030-48EF-9728-A621A2722181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3708" yWindow="2700" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -111,10 +111,7 @@
     <t>administrator@vsphere.local</t>
   </si>
   <si>
-    <t>R@ckware</t>
-  </si>
-  <si>
-    <t>NA</t>
+    <t>R@ckware4IT</t>
   </si>
 </sst>
 </file>
@@ -173,13 +170,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,7 +461,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +469,7 @@
     <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
@@ -495,40 +492,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -611,14 +608,14 @@
       <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
+      <c r="E3">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -630,9 +627,10 @@
     <mergeCell ref="G1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{0695EAEF-2BB0-4879-8A9C-85CCE587F892}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{22819FE3-187D-40E2-991C-EA1870DCA300}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{DA5A4927-21E8-44EC-AD04-54A16FA17957}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>